<commit_message>
Description: CONSULTA PARA VERIFICAR QUANTIDADE DE STATUS PROFISSIONAL
</commit_message>
<xml_diff>
--- a/Dashboard Excel/Projeto+2+-+Perfil+dos+leads.xlsx
+++ b/Dashboard Excel/Projeto+2+-+Perfil+dos+leads.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HD\ESTUDOS EM GERAL GRADE 1 SEMENTRES 2025\SQL PARA ANALISTA DE DADOS\Projeto de analise de perfil dos clientes\Dashboard Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D5B30EE-3C0B-4EEF-A7B8-A85508F15E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39C753B-E16D-4F41-95BD-EEADD5112D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="6" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>visitas (#)</t>
   </si>
@@ -104,6 +104,57 @@
   </si>
   <si>
     <t>veículos visitados (%)</t>
+  </si>
+  <si>
+    <t>Mulheres</t>
+  </si>
+  <si>
+    <t>Homens</t>
+  </si>
+  <si>
+    <t>Leads %</t>
+  </si>
+  <si>
+    <t>Funcionário(a) público(a)</t>
+  </si>
+  <si>
+    <t>0.017085507188657454</t>
+  </si>
+  <si>
+    <t>aposentado</t>
+  </si>
+  <si>
+    <t>0.04261420207893584</t>
+  </si>
+  <si>
+    <t>freelancer</t>
+  </si>
+  <si>
+    <t>0.052889402206380186</t>
+  </si>
+  <si>
+    <t>autônomo</t>
+  </si>
+  <si>
+    <t>0.07204587996335975</t>
+  </si>
+  <si>
+    <t>Empressário</t>
+  </si>
+  <si>
+    <t>0.07539129395834163</t>
+  </si>
+  <si>
+    <t>outros</t>
+  </si>
+  <si>
+    <t>0.09044565693576008</t>
+  </si>
+  <si>
+    <t>clt</t>
+  </si>
+  <si>
+    <t>0.6494484049543988</t>
   </si>
 </sst>
 </file>
@@ -178,7 +229,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -199,6 +250,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,13 +469,18 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>Output!$B$4:$B$5</c:f>
-              <c:numCache>
-                <c:formatCode>[$-416]mmm\-yy;@</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="2"/>
-              </c:numCache>
-            </c:numRef>
+                <c:pt idx="0">
+                  <c:v>Mulheres</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Homens</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -431,6 +488,12 @@
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>15105</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -622,7 +685,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>leads (%)</c:v>
+                  <c:v>Leads %</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -698,20 +761,61 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>Output!$E$4:$E$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="8"/>
-              </c:numCache>
-            </c:numRef>
+                <c:pt idx="2">
+                  <c:v>Funcionário(a) público(a)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>aposentado</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>freelancer</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>autônomo</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Empressário</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>outros</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Output!$F$4:$F$11</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>398263570831.17603</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>398263570831.17603</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0%">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0%">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0%">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0%">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0%">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0%">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -806,7 +910,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5534,6 +5638,157 @@
             <a:cs typeface="+mn-cs"/>
           </a:endParaRPr>
         </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>SELECT </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    CASE </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	    WHEN ibge.gender = 'male' THEN 'homens'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		WHEN ibge.gender = 'female' THEN 'mulheres'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		END AS "Gênero", </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		COUNT(*) AS "leads (#)"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>FROM sales.customers AS cus</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>LEFT JOIN temp_tables.ibge_genders AS ibge</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>     ON LOWER(cus.first_name) = LOWER(ibge.first_name)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>GROUP BY ibge.gender; </a:t>
+          </a:r>
+        </a:p>
       </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
@@ -6485,7 +6740,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="AE25" sqref="AE25"/>
     </sheetView>
   </sheetViews>
@@ -6506,14 +6761,15 @@
   </sheetPr>
   <dimension ref="B2:X321"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="3" width="12.85546875" customWidth="1"/>
-    <col min="5" max="6" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" customWidth="1"/>
     <col min="7" max="8" width="10.7109375" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
     <col min="10" max="10" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
@@ -6559,7 +6815,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>4</v>
@@ -6603,10 +6859,16 @@
       </c>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B4" s="5"/>
-      <c r="C4" s="4"/>
+      <c r="B4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="4">
+        <v>15105</v>
+      </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="8"/>
+      <c r="F4" s="12">
+        <v>398263570831.17603</v>
+      </c>
       <c r="H4" s="1"/>
       <c r="I4" s="8"/>
       <c r="J4"/>
@@ -6623,10 +6885,16 @@
       <c r="X4" s="1"/>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B5" s="5"/>
-      <c r="C5" s="4"/>
+      <c r="B5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="4">
+        <v>9999</v>
+      </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="8"/>
+      <c r="F5" s="12">
+        <v>398263570831.17603</v>
+      </c>
       <c r="H5" s="1"/>
       <c r="I5" s="8"/>
       <c r="J5"/>
@@ -6643,8 +6911,12 @@
       <c r="X5" s="1"/>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="E6" s="1"/>
-      <c r="F6" s="8"/>
+      <c r="E6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="H6" s="1"/>
       <c r="I6" s="8"/>
       <c r="J6"/>
@@ -6659,8 +6931,12 @@
       <c r="X6" s="1"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="E7" s="1"/>
-      <c r="F7" s="8"/>
+      <c r="E7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="H7" s="1"/>
       <c r="I7" s="8"/>
       <c r="J7"/>
@@ -6675,8 +6951,12 @@
       <c r="X7" s="1"/>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="E8" s="1"/>
-      <c r="F8" s="8"/>
+      <c r="E8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="H8" s="1"/>
       <c r="I8" s="8"/>
       <c r="J8"/>
@@ -6691,8 +6971,12 @@
       <c r="X8" s="1"/>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="E9" s="1"/>
-      <c r="F9" s="8"/>
+      <c r="E9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>31</v>
+      </c>
       <c r="J9"/>
       <c r="R9" s="1"/>
       <c r="S9" s="2"/>
@@ -6702,22 +6986,36 @@
       <c r="X9" s="1"/>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="E10" s="1"/>
-      <c r="F10" s="8"/>
+      <c r="E10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="J10"/>
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="E11" s="1"/>
-      <c r="F11" s="8"/>
+      <c r="E11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="J11"/>
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" t="s">
+        <v>37</v>
+      </c>
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
@@ -8298,7 +8596,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M68" sqref="M68"/>
+      <selection activeCell="AG21" sqref="AG21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Description: FAIXA ETÁRIA DE IDADE DOS CLIENTES
</commit_message>
<xml_diff>
--- a/Dashboard Excel/Projeto+2+-+Perfil+dos+leads.xlsx
+++ b/Dashboard Excel/Projeto+2+-+Perfil+dos+leads.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HD\ESTUDOS EM GERAL GRADE 1 SEMENTRES 2025\SQL PARA ANALISTA DE DADOS\Projeto de analise de perfil dos clientes\Dashboard Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39C753B-E16D-4F41-95BD-EEADD5112D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCD502D-5D82-4406-B9C3-89AD545C05A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="6" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>visitas (#)</t>
   </si>
@@ -118,43 +118,34 @@
     <t>Funcionário(a) público(a)</t>
   </si>
   <si>
-    <t>0.017085507188657454</t>
-  </si>
-  <si>
     <t>aposentado</t>
-  </si>
-  <si>
-    <t>0.04261420207893584</t>
   </si>
   <si>
     <t>freelancer</t>
   </si>
   <si>
-    <t>0.052889402206380186</t>
-  </si>
-  <si>
     <t>autônomo</t>
-  </si>
-  <si>
-    <t>0.07204587996335975</t>
   </si>
   <si>
     <t>Empressário</t>
   </si>
   <si>
-    <t>0.07539129395834163</t>
-  </si>
-  <si>
     <t>outros</t>
-  </si>
-  <si>
-    <t>0.09044565693576008</t>
   </si>
   <si>
     <t>clt</t>
   </si>
   <si>
-    <t>0.6494484049543988</t>
+    <t>80+</t>
+  </si>
+  <si>
+    <t>40-60</t>
+  </si>
+  <si>
+    <t>20-40</t>
+  </si>
+  <si>
+    <t>60-80</t>
   </si>
 </sst>
 </file>
@@ -229,7 +220,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -250,7 +241,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -764,24 +764,27 @@
             <c:strRef>
               <c:f>Output!$E$4:$E$11</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="2">
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
                   <c:v>Funcionário(a) público(a)</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="1">
                   <c:v>aposentado</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="2">
                   <c:v>freelancer</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="3">
                   <c:v>autônomo</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="4">
                   <c:v>Empressário</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="5">
                   <c:v>outros</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>clt</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -790,31 +793,28 @@
             <c:numRef>
               <c:f>Output!$F$4:$F$11</c:f>
               <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>398263570831.17603</c:v>
+                  <c:v>1.7085507188657399E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>398263570831.17603</c:v>
+                  <c:v>4.2614202078935799E-2</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="0%">
-                  <c:v>0</c:v>
+                <c:pt idx="2">
+                  <c:v>5.2889402206380103E-2</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="0%">
-                  <c:v>0</c:v>
+                <c:pt idx="3">
+                  <c:v>7.2045879963359705E-2</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="0%">
-                  <c:v>0</c:v>
+                <c:pt idx="4">
+                  <c:v>7.5391293958341599E-2</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="0%">
-                  <c:v>0</c:v>
+                <c:pt idx="5">
+                  <c:v>9.0445656935759997E-2</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="0%">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="0%">
-                  <c:v>0</c:v>
+                <c:pt idx="6" formatCode="0.00%">
+                  <c:v>0.64944840495439804</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -910,7 +910,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1163,20 +1163,43 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>Output!$H$4:$H$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-              </c:numCache>
-            </c:numRef>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>80+</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60-80</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40-60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20-40</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Output!$I$4:$I$8</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.44</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1272,7 +1295,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5892,6 +5915,263 @@
             <a:cs typeface="+mn-cs"/>
           </a:endParaRPr>
         </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>SELECT </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>     CASE </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>         WHEN professional_status = 'freelancer' THEN 'freelancer'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>         WHEN professional_status =  'retired' THEN 'aposentado'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>         WHEN professional_status =  'clt' THEN 'clt'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>         WHEN professional_status = 'other' THEN 'outros'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>         WHEN professional_status = 'civil_servant' THEN 'Funcionário(a) público(a)'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>         WHEN professional_status = 'student ' THEN 'estudante'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>         WHEN professional_status = 'self_employed' THEN 'autônomo'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>         WHEN professional_status = 'busine ' THEN 'Empressário'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>         WHEN professional_status = 'businessman' THEN 'Empressário'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>         END AS "status profissional", </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>         (COUNT(*)::float) /(SELECT COUNT(*) FROM sales.customers) AS "Leads %"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>FROM sales.customers</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>GROUP BY professional_status</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>ORDER BY "Leads %"; </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:br>
+            <a:rPr lang="pt-BR" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:endParaRPr lang="pt-BR" sz="1100" b="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
       </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
@@ -5994,6 +6274,160 @@
             <a:ea typeface="+mn-ea"/>
             <a:cs typeface="+mn-cs"/>
           </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>SELECT </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>      CASE </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	      WHEN datediff('years', birth_date, current_date) &lt;= 20 THEN '0-20'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		  WHEN datediff('years', birth_date, current_date) &lt; 40 THEN '20-40'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		  WHEN datediff('years', birth_date, current_date) &lt; 60 THEN '40-60'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		  WHEN datediff('years', birth_date, current_date) &lt; 80 THEN '60-80'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		  ELSE '80+' END "Faixa etária", </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		  COUNT(*)::float/(SELECT COUNT(*) FROM sales.customers) AS "leads (%)" </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>FROM sales.customers</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>GROUP BY "Faixa etária"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>ORDER BY "Faixa etária" DESC;  </a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -6741,7 +7175,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AE25" sqref="AE25"/>
+      <selection activeCell="AD16" sqref="AD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6761,15 +7195,15 @@
   </sheetPr>
   <dimension ref="B2:X321"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="3" width="12.85546875" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="32.85546875" customWidth="1"/>
+    <col min="6" max="6" width="36.140625" customWidth="1"/>
     <col min="7" max="8" width="10.7109375" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
     <col min="10" max="10" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
@@ -6817,10 +7251,10 @@
       <c r="F3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="13" t="s">
         <v>18</v>
       </c>
       <c r="J3"/>
@@ -6865,12 +7299,18 @@
       <c r="C4" s="4">
         <v>15105</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="12">
-        <v>398263570831.17603</v>
+      <c r="E4" s="1" t="s">
+        <v>24</v>
       </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="8"/>
+      <c r="F4" s="8">
+        <v>1.7085507188657399E-2</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="14">
+        <v>0.02</v>
+      </c>
       <c r="J4"/>
       <c r="K4" s="1"/>
       <c r="L4" s="8"/>
@@ -6891,12 +7331,18 @@
       <c r="C5" s="4">
         <v>9999</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="12">
-        <v>398263570831.17603</v>
+      <c r="E5" s="1" t="s">
+        <v>25</v>
       </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="8"/>
+      <c r="F5" s="8">
+        <v>4.2614202078935799E-2</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="14">
+        <v>0.2</v>
+      </c>
       <c r="J5"/>
       <c r="K5" s="1"/>
       <c r="L5" s="8"/>
@@ -6912,13 +7358,17 @@
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.25">
       <c r="E6" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
-      <c r="F6" s="8" t="s">
-        <v>25</v>
+      <c r="F6" s="8">
+        <v>5.2889402206380103E-2</v>
       </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="8"/>
+      <c r="H6" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="14">
+        <v>0.32</v>
+      </c>
       <c r="J6"/>
       <c r="K6" s="1"/>
       <c r="L6" s="8"/>
@@ -6932,13 +7382,17 @@
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.25">
       <c r="E7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="8"/>
+      <c r="F7" s="8">
+        <v>7.2045879963359705E-2</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="14">
+        <v>0.44</v>
+      </c>
       <c r="J7"/>
       <c r="K7" s="1"/>
       <c r="L7" s="8"/>
@@ -6954,11 +7408,11 @@
       <c r="E8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="8" t="s">
-        <v>29</v>
+      <c r="F8" s="8">
+        <v>7.5391293958341599E-2</v>
       </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="8"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="13"/>
       <c r="J8"/>
       <c r="K8" s="1"/>
       <c r="L8" s="8"/>
@@ -6972,10 +7426,10 @@
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.25">
       <c r="E9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
-      <c r="F9" s="8" t="s">
-        <v>31</v>
+      <c r="F9" s="8">
+        <v>9.0445656935759997E-2</v>
       </c>
       <c r="J9"/>
       <c r="R9" s="1"/>
@@ -6986,11 +7440,11 @@
       <c r="X9" s="1"/>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="E10" s="1" t="s">
-        <v>32</v>
+      <c r="E10" t="s">
+        <v>30</v>
       </c>
-      <c r="F10" s="8" t="s">
-        <v>33</v>
+      <c r="F10" s="15">
+        <v>0.64944840495439804</v>
       </c>
       <c r="J10"/>
       <c r="V10" s="1"/>
@@ -6998,34 +7452,28 @@
       <c r="X10" s="1"/>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="E11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>35</v>
-      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="8"/>
       <c r="J11"/>
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="E12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F12" t="s">
-        <v>37</v>
-      </c>
+      <c r="F12" s="15"/>
+      <c r="I12" s="15"/>
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="I13" s="15"/>
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
       <c r="X13" s="1"/>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="I14" s="15"/>
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
@@ -7061,21 +7509,25 @@
       <c r="X20" s="1"/>
     </row>
     <row r="21" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="M21" s="15"/>
       <c r="V21" s="1"/>
       <c r="W21" s="1"/>
       <c r="X21" s="1"/>
     </row>
     <row r="22" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="M22" s="15"/>
       <c r="V22" s="1"/>
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
     </row>
     <row r="23" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="M23" s="15"/>
       <c r="V23" s="1"/>
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
     </row>
     <row r="24" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="M24" s="15"/>
       <c r="V24" s="1"/>
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
@@ -8595,8 +9047,8 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AG21" sqref="AG21"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AB27" sqref="AB27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Description: CONSULTA faixa salarioa baseado na ledas e ordenada
</commit_message>
<xml_diff>
--- a/Dashboard Excel/Projeto+2+-+Perfil+dos+leads.xlsx
+++ b/Dashboard Excel/Projeto+2+-+Perfil+dos+leads.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HD\ESTUDOS EM GERAL GRADE 1 SEMENTRES 2025\SQL PARA ANALISTA DE DADOS\Projeto de analise de perfil dos clientes\Dashboard Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCD502D-5D82-4406-B9C3-89AD545C05A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9584AD04-6F66-4198-BDC0-BC09BCA9953C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>visitas (#)</t>
   </si>
@@ -50,9 +50,6 @@
   </si>
   <si>
     <t>status profissional</t>
-  </si>
-  <si>
-    <t>faixa salarial</t>
   </si>
   <si>
     <t>faixa etária</t>
@@ -146,6 +143,27 @@
   </si>
   <si>
     <t>60-80</t>
+  </si>
+  <si>
+    <t>Ordem</t>
+  </si>
+  <si>
+    <t>Faixa Salarial</t>
+  </si>
+  <si>
+    <t>20000+</t>
+  </si>
+  <si>
+    <t>15000-20000</t>
+  </si>
+  <si>
+    <t>10000-15000</t>
+  </si>
+  <si>
+    <t>5000-10000</t>
+  </si>
+  <si>
+    <t>0-5000</t>
   </si>
 </sst>
 </file>
@@ -1528,13 +1546,27 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>Output!$K$4:$K$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="5"/>
-              </c:numCache>
-            </c:numRef>
+                <c:pt idx="0">
+                  <c:v>20000+</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15000-20000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000-15000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5000-10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0-5000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1542,6 +1574,21 @@
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.6010195547413199E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7722728901987301E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.5384125214066598E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.71026325222031905</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.16061969811621299</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5573,7 +5620,7 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>166688</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>571500</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5589,7 +5636,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="557212" y="314325"/>
-          <a:ext cx="3943351" cy="3419475"/>
+          <a:ext cx="3895726" cy="3876675"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5827,7 +5874,7 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>32218</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>530679</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5842,8 +5889,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4658565" y="314325"/>
-          <a:ext cx="3845300" cy="3419475"/>
+          <a:off x="4708991" y="314325"/>
+          <a:ext cx="3895727" cy="3835854"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6187,7 +6234,7 @@
       <xdr:col>20</xdr:col>
       <xdr:colOff>469247</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>489857</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -6202,8 +6249,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8726300" y="314325"/>
-          <a:ext cx="3845300" cy="3419475"/>
+          <a:off x="8827153" y="314325"/>
+          <a:ext cx="3888523" cy="3795032"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6441,10 +6488,10 @@
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>233924</xdr:colOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>108857</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>462643</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -6459,8 +6506,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12726800" y="314325"/>
-          <a:ext cx="3845300" cy="3419475"/>
+          <a:off x="12878079" y="314325"/>
+          <a:ext cx="4375778" cy="3767818"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6519,6 +6566,255 @@
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>-- Colunas: faixa salarial, leads (%), ordem</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>SELECT </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>      CASE </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>          WHEN income &lt; 5000 THEN '0-5000'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>          WHEN income &lt; 10000 THEN '5000-10000'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>          WHEN income &lt; 15000 THEN '10000-15000'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>          WHEN income &lt; 20000 THEN '15000-20000'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>          ELSE '20000+' END "Faixa Salarial", </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>          COUNT(*)::float/(SELECT COUNT(*) FROM sales.customers) AS "leads (%)",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>      CASE </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>          WHEN income &lt; 5000 THEN 1</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>          WHEN income &lt; 10000 THEN 2</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>          WHEN income &lt; 15000 THEN 3</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>          WHEN income &lt; 20000 THEN 4</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>          ELSE 5 END "Ordem"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>FROM sales.customers</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>GROUP BY "Faixa Salarial", "Ordem"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>ORDER BY "Ordem" DESC;  </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -7196,7 +7492,7 @@
   <dimension ref="B2:X321"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7207,7 +7503,7 @@
     <col min="7" max="8" width="10.7109375" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
     <col min="10" max="10" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.7109375" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1"/>
     <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
@@ -7217,25 +7513,25 @@
   <sheetData>
     <row r="2" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="H2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="K2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="O2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="R2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="R2" s="11" t="s">
+      <c r="V2" s="11" t="s">
         <v>15</v>
-      </c>
-      <c r="V2" s="11" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="2:24" x14ac:dyDescent="0.25">
@@ -7243,50 +7539,50 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J3"/>
       <c r="K3" s="1" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="L3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>5</v>
+      <c r="S3" s="1" t="s">
+        <v>19</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>6</v>
+      <c r="T3" s="1" t="s">
+        <v>4</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="R3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="V3" s="1" t="s">
+      <c r="W3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="X3" s="1" t="s">
         <v>0</v>
@@ -7294,27 +7590,33 @@
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="4">
         <v>15105</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4" s="8">
         <v>1.7085507188657399E-2</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I4" s="14">
         <v>0.02</v>
       </c>
       <c r="J4"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="1"/>
+      <c r="K4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L4" s="13">
+        <v>1.6010195547413199E-2</v>
+      </c>
+      <c r="M4" s="1">
+        <v>5</v>
+      </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="R4" s="1"/>
@@ -7326,27 +7628,33 @@
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="4">
         <v>9999</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5" s="8">
         <v>4.2614202078935799E-2</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I5" s="14">
         <v>0.2</v>
       </c>
       <c r="J5"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="1"/>
+      <c r="K5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" s="13">
+        <v>1.7722728901987301E-2</v>
+      </c>
+      <c r="M5" s="1">
+        <v>4</v>
+      </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="R5" s="1"/>
@@ -7358,21 +7666,27 @@
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.25">
       <c r="E6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6" s="8">
         <v>5.2889402206380103E-2</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I6" s="14">
         <v>0.32</v>
       </c>
       <c r="J6"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="1"/>
+      <c r="K6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" s="13">
+        <v>9.5384125214066598E-2</v>
+      </c>
+      <c r="M6" s="1">
+        <v>3</v>
+      </c>
       <c r="R6" s="1"/>
       <c r="S6" s="2"/>
       <c r="T6" s="1"/>
@@ -7382,21 +7696,27 @@
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.25">
       <c r="E7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="8">
         <v>7.2045879963359705E-2</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I7" s="14">
         <v>0.44</v>
       </c>
       <c r="J7"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="1"/>
+      <c r="K7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L7" s="13">
+        <v>0.71026325222031905</v>
+      </c>
+      <c r="M7" s="1">
+        <v>2</v>
+      </c>
       <c r="R7" s="1"/>
       <c r="S7" s="2"/>
       <c r="T7" s="1"/>
@@ -7406,7 +7726,7 @@
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.25">
       <c r="E8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8" s="8">
         <v>7.5391293958341599E-2</v>
@@ -7414,9 +7734,15 @@
       <c r="H8" s="12"/>
       <c r="I8" s="13"/>
       <c r="J8"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="1"/>
+      <c r="K8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L8" s="13">
+        <v>0.16061969811621299</v>
+      </c>
+      <c r="M8" s="1">
+        <v>1</v>
+      </c>
       <c r="R8" s="1"/>
       <c r="S8" s="2"/>
       <c r="T8" s="1"/>
@@ -7426,7 +7752,7 @@
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.25">
       <c r="E9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F9" s="8">
         <v>9.0445656935759997E-2</v>
@@ -7441,7 +7767,7 @@
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F10" s="15">
         <v>0.64944840495439804</v>
@@ -9045,14 +9371,16 @@
   <sheetPr>
     <tabColor rgb="FF404040"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AB27" sqref="AB27"/>
+      <selection activeCell="AE16" sqref="AE16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="20" ht="62.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Description: QUERY DE CONSULTA PARA LEVANTAR O NUMERO DE LEADS BASEADO EM CARROS SEMINOVOS E NOVOS
</commit_message>
<xml_diff>
--- a/Dashboard Excel/Projeto+2+-+Perfil+dos+leads.xlsx
+++ b/Dashboard Excel/Projeto+2+-+Perfil+dos+leads.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HD\ESTUDOS EM GERAL GRADE 1 SEMENTRES 2025\SQL PARA ANALISTA DE DADOS\Projeto de analise de perfil dos clientes\Dashboard Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9584AD04-6F66-4198-BDC0-BC09BCA9953C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9683F830-0664-4EAE-9D47-6D2F0F22CC06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>visitas (#)</t>
   </si>
@@ -164,6 +164,12 @@
   </si>
   <si>
     <t>0-5000</t>
+  </si>
+  <si>
+    <t>novo</t>
+  </si>
+  <si>
+    <t>seminovo</t>
   </si>
 </sst>
 </file>
@@ -1957,13 +1963,18 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>Output!$O$4:$O$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="2"/>
-              </c:numCache>
-            </c:numRef>
+                <c:pt idx="0">
+                  <c:v>novo</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>seminovo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1971,6 +1982,12 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1162</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29418</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6842,8 +6859,8 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>193104</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>100693</xdr:rowOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -6858,8 +6875,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="590830" y="3920218"/>
-          <a:ext cx="3888524" cy="3419475"/>
+          <a:off x="590830" y="4518932"/>
+          <a:ext cx="3888524" cy="5087711"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6945,6 +6962,283 @@
             <a:cs typeface="+mn-cs"/>
           </a:endParaRPr>
         </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>WITH classificacao_veiculos AS ( </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    SELECT </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>        fun.visit_page_date, </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>        pro.model_year, </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>		EXTRACT('year' FROM current_date) - pro.model_year::int AS "Exemplo de idade do veículo", </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>        EXTRACT('year' FROM visit_page_date) - pro.model_year::int AS idade_veiculo,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>        CASE </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            WHEN (EXTRACT('year' FROM visit_page_date) - pro.model_year::int) &lt;= 2 THEN 'novo'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            ELSE 'seminovo'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>        END AS "classificação do veículo"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    FROM sales.funnel AS fun </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    LEFT JOIN sales.products AS pro </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>         ON fun.product_id = pro.product_id</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>SELECT </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>     "classificação do veículo", </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	 COUNT(*) AS "veículos visitados (#)"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	 FROM classificacao_veiculos</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	 GROUP BY "classificação do veículo";</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
       </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
@@ -6959,8 +7253,8 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>29818</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>100693</xdr:rowOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>40822</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -6975,8 +7269,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4713794" y="3920218"/>
-          <a:ext cx="3888524" cy="3419475"/>
+          <a:off x="4713794" y="4518932"/>
+          <a:ext cx="3888524" cy="5074104"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7062,8 +7356,8 @@
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>492460</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>100693</xdr:rowOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -7078,8 +7372,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8850365" y="3920218"/>
-          <a:ext cx="3888524" cy="3419475"/>
+          <a:off x="8850365" y="4518932"/>
+          <a:ext cx="3888524" cy="5087711"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7492,7 +7786,7 @@
   <dimension ref="B2:X321"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7617,8 +7911,12 @@
       <c r="M4" s="1">
         <v>5</v>
       </c>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
+      <c r="O4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P4" s="1">
+        <v>1162</v>
+      </c>
       <c r="R4" s="1"/>
       <c r="S4" s="2"/>
       <c r="T4" s="1"/>
@@ -7655,8 +7953,12 @@
       <c r="M5" s="1">
         <v>4</v>
       </c>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
+      <c r="O5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P5" s="1">
+        <v>29418</v>
+      </c>
       <c r="R5" s="1"/>
       <c r="S5" s="2"/>
       <c r="T5" s="1"/>
@@ -9374,7 +9676,7 @@
   <dimension ref="A20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AE16" sqref="AE16"/>
+      <selection activeCell="Z42" sqref="Z42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Descriptino: query leads e idade de carro
</commit_message>
<xml_diff>
--- a/Dashboard Excel/Projeto+2+-+Perfil+dos+leads.xlsx
+++ b/Dashboard Excel/Projeto+2+-+Perfil+dos+leads.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HD\ESTUDOS EM GERAL GRADE 1 SEMENTRES 2025\SQL PARA ANALISTA DE DADOS\Projeto de analise de perfil dos clientes\Dashboard Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9683F830-0664-4EAE-9D47-6D2F0F22CC06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB6CDA2-A98C-411A-A6DB-644D2E82DDFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="6" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>visitas (#)</t>
   </si>
@@ -170,6 +170,24 @@
   </si>
   <si>
     <t>seminovo</t>
+  </si>
+  <si>
+    <t>até 2 anos</t>
+  </si>
+  <si>
+    <t>até 10 á 14 anos</t>
+  </si>
+  <si>
+    <t>até 4 á 8 anos</t>
+  </si>
+  <si>
+    <t>acima de 10 anos</t>
+  </si>
+  <si>
+    <t>até 2 á 4 anos</t>
+  </si>
+  <si>
+    <t>até 8 á 10 anos</t>
   </si>
 </sst>
 </file>
@@ -2235,13 +2253,30 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>Output!$R$4:$R$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="6"/>
-              </c:numCache>
-            </c:numRef>
+                <c:pt idx="0">
+                  <c:v>até 2 anos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>até 2 á 4 anos</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>até 4 á 8 anos</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>até 8 á 10 anos</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>até 10 á 14 anos</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>acima de 10 anos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -2249,6 +2284,24 @@
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3.7998691955526402E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.10775016350555899</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.18103335513407401</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.19630477436232799</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.247645519947678</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.22926749509483299</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7764,8 +7817,8 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AD16" sqref="AD16"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7786,7 +7839,7 @@
   <dimension ref="B2:X321"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7917,9 +7970,15 @@
       <c r="P4" s="1">
         <v>1162</v>
       </c>
-      <c r="R4" s="1"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="1"/>
+      <c r="R4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="S4" s="2">
+        <v>3.7998691955526402E-2</v>
+      </c>
+      <c r="T4" s="1">
+        <v>1</v>
+      </c>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
@@ -7959,9 +8018,15 @@
       <c r="P5" s="1">
         <v>29418</v>
       </c>
-      <c r="R5" s="1"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="1"/>
+      <c r="R5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="S5" s="2">
+        <v>0.10775016350555899</v>
+      </c>
+      <c r="T5" s="1">
+        <v>2</v>
+      </c>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
@@ -7989,9 +8054,15 @@
       <c r="M6" s="1">
         <v>3</v>
       </c>
-      <c r="R6" s="1"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="1"/>
+      <c r="R6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="S6" s="2">
+        <v>0.18103335513407401</v>
+      </c>
+      <c r="T6" s="1">
+        <v>3</v>
+      </c>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
@@ -8019,9 +8090,15 @@
       <c r="M7" s="1">
         <v>2</v>
       </c>
-      <c r="R7" s="1"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="1"/>
+      <c r="R7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="S7" s="2">
+        <v>0.19630477436232799</v>
+      </c>
+      <c r="T7" s="1">
+        <v>4</v>
+      </c>
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
@@ -8045,9 +8122,15 @@
       <c r="M8" s="1">
         <v>1</v>
       </c>
-      <c r="R8" s="1"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="1"/>
+      <c r="R8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S8" s="2">
+        <v>0.247645519947678</v>
+      </c>
+      <c r="T8" s="1">
+        <v>5</v>
+      </c>
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
@@ -8060,9 +8143,15 @@
         <v>9.0445656935759997E-2</v>
       </c>
       <c r="J9"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="1"/>
+      <c r="R9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="S9" s="2">
+        <v>0.22926749509483299</v>
+      </c>
+      <c r="T9" s="1">
+        <v>6</v>
+      </c>
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
@@ -9675,8 +9764,8 @@
   </sheetPr>
   <dimension ref="A20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Z42" sqref="Z42"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AG23" sqref="AG23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>